<commit_message>
MOD: Se agregaron nuevos datos a los excels
</commit_message>
<xml_diff>
--- a/python/Datos_Especializacion_Maestria.xlsx
+++ b/python/Datos_Especializacion_Maestria.xlsx
@@ -406,40 +406,45 @@
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>Periodo grado maestria</t>
+          <t>Periodo ultima matricula</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
+          <t>Mas de dos semestres desde ultima matricula</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
           <t>Linkedin</t>
         </is>
       </c>
-      <c r="M1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>Ultimo rol</t>
         </is>
       </c>
-      <c r="N1" t="inlineStr">
+      <c r="O1" t="inlineStr">
         <is>
           <t>Trabajo de grado</t>
         </is>
       </c>
-      <c r="O1" t="inlineStr">
+      <c r="P1" t="inlineStr">
         <is>
           <t>Año de sustentacion</t>
         </is>
       </c>
-      <c r="P1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>Director</t>
         </is>
       </c>
-      <c r="Q1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>Pendiente de especializacion</t>
         </is>
       </c>
-      <c r="R1" t="inlineStr">
+      <c r="S1" t="inlineStr">
         <is>
           <t>Pendiente de maestria</t>
         </is>
@@ -498,40 +503,45 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>2019-2</t>
+          <t>2018-1</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M2" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/leonidas-andrade-a8183269/</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
+      <c r="N2" t="inlineStr">
         <is>
           <t>Ingeniero de sistemas alcaldía de cali</t>
         </is>
       </c>
-      <c r="N2" t="inlineStr">
+      <c r="O2" t="inlineStr">
         <is>
           <t>IMPLEMENTACIÓN DE UNA PLATAFORMA COLABORATIVA DEL INTERNET DE LAS COSAS PARA LA CAPTURA DE VARIABLE AMBIENTALES PARA EL MUNICIPIO SANTIAGO DE CALI</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
+      <c r="P2" t="inlineStr">
         <is>
           <t>02 DE MAYO DE 2019</t>
         </is>
       </c>
-      <c r="P2" t="inlineStr">
+      <c r="Q2" t="inlineStr">
         <is>
           <t>LUIS EDUARDO TOBÓN LLANO</t>
         </is>
       </c>
-      <c r="Q2" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -588,26 +598,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K3" t="inlineStr"/>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>2018-1</t>
+        </is>
+      </c>
       <c r="L3" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/cristian-alejandro-chaparro-cuadros-70899062/</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
+      <c r="N3" t="inlineStr">
         <is>
           <t>Arquitecto soluciones intergrupo</t>
         </is>
       </c>
-      <c r="N3" t="inlineStr"/>
       <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr"/>
-      <c r="Q3" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q3" t="inlineStr"/>
       <c r="R3" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -666,40 +685,45 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>2019-1</t>
+          <t>2018-1</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/carlos-felipe-domínguez-illera-71b243188/</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N4" t="inlineStr">
         <is>
           <t>Jefe de Tecnología de la Información Club Noel</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O4" t="inlineStr">
         <is>
           <t>DEFINICIÓN Y ANÁLISIS DE REQUISITOS DEL SISTEMA DE INFORMACIÓN PARA EL PROGRAMA DE ALIMENTACIÓN ESCOLAR GOBERNACIÓN DEL CAUCA E IMPLEMENTACIÓN DEL SISTEMA DE PRIORIZACIÓN, SEGUIMIENTO Y CONTROL DEL PROGRAMA.</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr">
+      <c r="P4" t="inlineStr">
         <is>
           <t>13 DE DICIEMBRE DE 2018</t>
         </is>
       </c>
-      <c r="P4" t="inlineStr">
+      <c r="Q4" t="inlineStr">
         <is>
           <t>JUAN CARLOS MARTÍNEZ ARIAS</t>
         </is>
       </c>
-      <c r="Q4" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -758,36 +782,41 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>2019-1</t>
+          <t>2018-2</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
           <t>NO encontada</t>
         </is>
       </c>
-      <c r="M5" t="inlineStr"/>
-      <c r="N5" t="inlineStr">
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr">
         <is>
           <t>DISEÑO DE UNA ARQUITECTURA Y UN PROTOTIPO DE UN JUEGO DE MESA INTEGRADO CON REALIDAD AUMENTADA, PARA LA PROMOCIÓN DEL CUIDADO Y LA UTILIZACIÓN DEL AGUA EN POTRERITO</t>
         </is>
       </c>
-      <c r="O5" t="inlineStr">
+      <c r="P5" t="inlineStr">
         <is>
           <t>14 DE FEBRRERO DE 2019</t>
         </is>
       </c>
-      <c r="P5" t="inlineStr">
+      <c r="Q5" t="inlineStr">
         <is>
           <t>ANDRÉS NAVARRO NEWBALL</t>
         </is>
       </c>
-      <c r="Q5" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R5" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -846,40 +875,45 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>2020-1</t>
+          <t>2018-1</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/ricardo-jaramillo-a498a0173/</t>
         </is>
       </c>
-      <c r="M6" t="inlineStr">
+      <c r="N6" t="inlineStr">
         <is>
           <t>Analista de desarrollo en Codesa S.A.</t>
         </is>
       </c>
-      <c r="N6" t="inlineStr">
+      <c r="O6" t="inlineStr">
         <is>
           <t>DISEÑO DE ARQUITECTURA DE SOFTWARE PARA UNA EMPRESA DE TECNOLOGÍA DE APOYO A NEGOCIOS DE JUEGOS DE AZAR</t>
         </is>
       </c>
-      <c r="O6" t="inlineStr">
+      <c r="P6" t="inlineStr">
         <is>
           <t>05 DE SEPTIEMBRE DE 2019</t>
         </is>
       </c>
-      <c r="P6" t="inlineStr">
+      <c r="Q6" t="inlineStr">
         <is>
           <t xml:space="preserve">MARÍA CONSTANZA PABÓN BURBANO </t>
         </is>
       </c>
-      <c r="Q6" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R6" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -936,26 +970,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K7" t="inlineStr"/>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>2018-1</t>
+        </is>
+      </c>
       <c r="L7" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/jlopez0313/</t>
         </is>
       </c>
-      <c r="M7" t="inlineStr">
+      <c r="N7" t="inlineStr">
         <is>
           <t>Coordinador Nacional de Sistemas at DELTEC S.A.</t>
         </is>
       </c>
-      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr"/>
       <c r="P7" t="inlineStr"/>
-      <c r="Q7" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -1012,18 +1055,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>2017-1</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
       <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr"/>
       <c r="O8" t="inlineStr"/>
       <c r="P8" t="inlineStr"/>
-      <c r="Q8" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q8" t="inlineStr"/>
       <c r="R8" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -1078,40 +1130,45 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>2019-1</t>
+          <t>2018-1</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/orvalen/</t>
         </is>
       </c>
-      <c r="M9" t="inlineStr">
+      <c r="N9" t="inlineStr">
         <is>
           <t>Líder Operación Internet</t>
         </is>
       </c>
-      <c r="N9" t="inlineStr">
+      <c r="O9" t="inlineStr">
         <is>
           <t>ARQUITECTURA TECNOLÓGICA DE AUTOMATIZACIÓN PARA LA SUPERVISIÓN, CONTROL Y MEDIDA DE NUEVOS NEGOCIOS EN LOS MERCADOS DE CIUDADES, EMPRESAS Y HOGARES DE CELSIA</t>
         </is>
       </c>
-      <c r="O9" t="inlineStr">
+      <c r="P9" t="inlineStr">
         <is>
           <t>15 DE FEBRERO DE 2019</t>
         </is>
       </c>
-      <c r="P9" t="inlineStr">
+      <c r="Q9" t="inlineStr">
         <is>
           <t>JAIME ALBERTO SÁNCHEZ</t>
         </is>
       </c>
-      <c r="Q9" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R9" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -1164,18 +1221,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr"/>
-      <c r="L10" t="inlineStr"/>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
       <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr"/>
       <c r="O10" t="inlineStr"/>
       <c r="P10" t="inlineStr"/>
-      <c r="Q10" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q10" t="inlineStr"/>
       <c r="R10" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -1234,40 +1300,45 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>2019-2</t>
+          <t>2018-2</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/davidportocarrero/</t>
         </is>
       </c>
-      <c r="M11" t="inlineStr">
+      <c r="N11" t="inlineStr">
         <is>
           <t>Desarrollador Comunity SAS</t>
         </is>
       </c>
-      <c r="N11" t="inlineStr">
+      <c r="O11" t="inlineStr">
         <is>
           <t>HERRAMIENTA DE PROGRAMACIÓN VISUAL PARA CREAR SERVICIOS WEB</t>
         </is>
       </c>
-      <c r="O11" t="inlineStr">
+      <c r="P11" t="inlineStr">
         <is>
           <t>25 DE JULIO DE 2019</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr">
+      <c r="Q11" t="inlineStr">
         <is>
           <t>SIMENA DINAS</t>
         </is>
       </c>
-      <c r="Q11" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R11" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -1322,36 +1393,41 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>2019-1</t>
+          <t>2018-2</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/gasalaza/</t>
         </is>
       </c>
-      <c r="M12" t="inlineStr"/>
-      <c r="N12" t="inlineStr">
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr">
         <is>
           <t>DEFINICIÓN DE UNA PLATAFORMA MODULAR Y ESCALABLE PARA LA GESTIÓN DE PROPIEDADES HORIZONTALES EN COLOMBIA</t>
         </is>
       </c>
-      <c r="O12" t="inlineStr">
+      <c r="P12" t="inlineStr">
         <is>
           <t>14 DE MARZO DE 2019</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr">
+      <c r="Q12" t="inlineStr">
         <is>
           <t>GERARDO SARRIA</t>
         </is>
       </c>
-      <c r="Q12" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R12" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -1410,36 +1486,41 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>2019-2</t>
+          <t>2018-2</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/martin-v-a-sierra-galvis-46153a126/</t>
         </is>
       </c>
-      <c r="M13" t="inlineStr"/>
-      <c r="N13" t="inlineStr">
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr">
         <is>
           <t>DERIVACIÓN DE PRODUCTOS EN UNA HERRAMIENTA DE SOFTWARE PARA LA REHABILITACIÓN DE NIÑOS CON DISCAPACIDAD AUDITIVA, SIGUIENDO EL PARADIGMA DE LAS LÍNEAS DE PRODUCTOS DE SOFTWARE.</t>
         </is>
       </c>
-      <c r="O13" t="inlineStr">
+      <c r="P13" t="inlineStr">
         <is>
           <t>20 DE MAYO DE 2019</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr">
+      <c r="Q13" t="inlineStr">
         <is>
           <t>JUAN CARLOS MARTÍNEZ ARIAS</t>
         </is>
       </c>
-      <c r="Q13" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R13" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -1496,22 +1577,31 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr"/>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L14" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
           <t>NO encontada</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr"/>
       <c r="O14" t="inlineStr"/>
       <c r="P14" t="inlineStr"/>
-      <c r="Q14" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -1570,40 +1660,45 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>2020-2</t>
+          <t>2018-2</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/andres-felipe-tobar-vega-b005b770/</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr">
+      <c r="N15" t="inlineStr">
         <is>
           <t>Director área de arquitectura e ingeniería de software en Corporación Talentum</t>
         </is>
       </c>
-      <c r="N15" t="inlineStr">
+      <c r="O15" t="inlineStr">
         <is>
           <t>DISEÑO DE UN SISTEMA DE GESTIÓN DEL APRENDIZAJE CENTRADO EN EL USUARIO EN EL CONTEXTO DE LA CIBERCULTURA Y LA BRECHA DIGITAL”</t>
         </is>
       </c>
-      <c r="O15" t="inlineStr">
+      <c r="P15" t="inlineStr">
         <is>
           <t>13 DE ENERO DE 2020</t>
         </is>
       </c>
-      <c r="P15" t="inlineStr">
+      <c r="Q15" t="inlineStr">
         <is>
           <t>SIMENA DINAS</t>
         </is>
       </c>
-      <c r="Q15" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R15" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -1660,27 +1755,36 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K16" t="inlineStr"/>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>2019-1</t>
+        </is>
+      </c>
       <c r="L16" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/jhonfgomezg/</t>
         </is>
       </c>
-      <c r="M16" t="inlineStr">
+      <c r="N16" t="inlineStr">
         <is>
           <t>Director de Tecnología
 Desarrollador Senior Python y .NET</t>
         </is>
       </c>
-      <c r="N16" t="inlineStr"/>
       <c r="O16" t="inlineStr"/>
       <c r="P16" t="inlineStr"/>
-      <c r="Q16" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q16" t="inlineStr"/>
       <c r="R16" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -1733,18 +1837,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K17" t="inlineStr"/>
-      <c r="L17" t="inlineStr"/>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>2019-2</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
       <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr"/>
       <c r="O17" t="inlineStr"/>
       <c r="P17" t="inlineStr"/>
-      <c r="Q17" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q17" t="inlineStr"/>
       <c r="R17" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -1801,26 +1914,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K18" t="inlineStr"/>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>2019-1</t>
+        </is>
+      </c>
       <c r="L18" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/edwin-andres-leon-castro-00ab8047/</t>
         </is>
       </c>
-      <c r="M18" t="inlineStr">
+      <c r="N18" t="inlineStr">
         <is>
           <t>Ingeniero de Soporte I+D INELCA</t>
         </is>
       </c>
-      <c r="N18" t="inlineStr"/>
       <c r="O18" t="inlineStr"/>
       <c r="P18" t="inlineStr"/>
-      <c r="Q18" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q18" t="inlineStr"/>
       <c r="R18" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -1877,26 +1999,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K19" t="inlineStr"/>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>2018-1</t>
+        </is>
+      </c>
       <c r="L19" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/alejandro-romero-80a2926b/</t>
         </is>
       </c>
-      <c r="M19" t="inlineStr">
+      <c r="N19" t="inlineStr">
         <is>
           <t>Full Stack Developer at PRAGMA S.A</t>
         </is>
       </c>
-      <c r="N19" t="inlineStr"/>
       <c r="O19" t="inlineStr"/>
       <c r="P19" t="inlineStr"/>
-      <c r="Q19" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q19" t="inlineStr"/>
       <c r="R19" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -1949,18 +2080,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K20" t="inlineStr"/>
-      <c r="L20" t="inlineStr"/>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>2019-1</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
       <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr"/>
       <c r="O20" t="inlineStr"/>
       <c r="P20" t="inlineStr"/>
-      <c r="Q20" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q20" t="inlineStr"/>
       <c r="R20" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -2019,41 +2159,46 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>2020-2</t>
+          <t>2019-2</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/héctor-andrés-espinal-209134122/</t>
         </is>
       </c>
-      <c r="M21" t="inlineStr">
+      <c r="N21" t="inlineStr">
         <is>
           <t>Ingeniero de Aplicaciones Backoffice en Carvajal Tecnología y Servicios</t>
         </is>
       </c>
-      <c r="N21" t="inlineStr">
+      <c r="O21" t="inlineStr">
         <is>
           <t xml:space="preserve">"ARQUITECTURA DE SOFTWARE ORIENTADO A LA GESTIÓN DOCUMENTAL PARA MIPYMES DEL VALLE DEL CAUCA"
 </t>
         </is>
       </c>
-      <c r="O21" t="inlineStr">
+      <c r="P21" t="inlineStr">
         <is>
           <t>02 DE JUNIO DE 2020</t>
         </is>
       </c>
-      <c r="P21" t="inlineStr">
+      <c r="Q21" t="inlineStr">
         <is>
           <t>CARLO ALBERTO LLANO RODRIGUEZ</t>
         </is>
       </c>
-      <c r="Q21" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R21" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -2110,26 +2255,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr"/>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>2019-2</t>
+        </is>
+      </c>
       <c r="L22" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/cristhian-david-bastidas-baca-b72aba158/</t>
         </is>
       </c>
-      <c r="M22" t="inlineStr">
+      <c r="N22" t="inlineStr">
         <is>
           <t>Desarrollador banco de occidente</t>
         </is>
       </c>
-      <c r="N22" t="inlineStr"/>
       <c r="O22" t="inlineStr"/>
       <c r="P22" t="inlineStr"/>
-      <c r="Q22" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q22" t="inlineStr"/>
       <c r="R22" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -2188,40 +2342,45 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>2020-1</t>
+          <t>2019-2</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/luis-fernando-benavides-rengifo-8a5b054/</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr">
+      <c r="N23" t="inlineStr">
         <is>
           <t>Desarrollador de Software (Desarrollador de back-end proyecto Nequi)</t>
         </is>
       </c>
-      <c r="N23" t="inlineStr">
+      <c r="O23" t="inlineStr">
         <is>
           <t>“BUSCANDO LA EXCELENCIA EDUCATIVA: ESTUDIO DE FACTIBILIDAD PARA LA IMPLEMENTACIÓN DE UNA PLATAFORMA LOW-CODE EN LA PONTIFICIA UNIVERSIDAD JAVERIANA, SECCIONAL CALI”</t>
         </is>
       </c>
-      <c r="O23" t="inlineStr">
+      <c r="P23" t="inlineStr">
         <is>
           <t>27  DE ENERO DE 2020</t>
         </is>
       </c>
-      <c r="P23" t="inlineStr">
+      <c r="Q23" t="inlineStr">
         <is>
           <t>JOSÉ DAVID ESCOBAR ARDILA</t>
         </is>
       </c>
-      <c r="Q23" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R23" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -2278,26 +2437,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr"/>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L24" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/milton-marulanda/</t>
         </is>
       </c>
-      <c r="M24" t="inlineStr">
+      <c r="N24" t="inlineStr">
         <is>
           <t>Arquitecto de Software en GTC Corporation</t>
         </is>
       </c>
-      <c r="N24" t="inlineStr"/>
       <c r="O24" t="inlineStr"/>
       <c r="P24" t="inlineStr"/>
-      <c r="Q24" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q24" t="inlineStr"/>
       <c r="R24" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -2354,26 +2522,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr"/>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L25" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/marco-antonio-ortega-piedrahita-674370184/</t>
         </is>
       </c>
-      <c r="M25" t="inlineStr">
+      <c r="N25" t="inlineStr">
         <is>
           <t>Analista Devops en TCM ideas</t>
         </is>
       </c>
-      <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr"/>
       <c r="P25" t="inlineStr"/>
-      <c r="Q25" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -2430,26 +2607,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K26" t="inlineStr"/>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L26" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/luis-felipe-rojas-46121613a/</t>
         </is>
       </c>
-      <c r="M26" t="inlineStr">
+      <c r="N26" t="inlineStr">
         <is>
           <t>Senior Full Stack Engineer at Paladin Cyber</t>
         </is>
       </c>
-      <c r="N26" t="inlineStr"/>
       <c r="O26" t="inlineStr"/>
       <c r="P26" t="inlineStr"/>
-      <c r="Q26" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q26" t="inlineStr"/>
       <c r="R26" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -2506,26 +2692,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K27" t="inlineStr"/>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L27" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/edward-andres-toro-pretelt/</t>
         </is>
       </c>
-      <c r="M27" t="inlineStr">
+      <c r="N27" t="inlineStr">
         <is>
           <t>Consultor ABAP,Portals, XI/PI, SMP, REX, MOVILIDAD, ABAP CRM, ABAP HCM</t>
         </is>
       </c>
-      <c r="N27" t="inlineStr"/>
       <c r="O27" t="inlineStr"/>
       <c r="P27" t="inlineStr"/>
-      <c r="Q27" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q27" t="inlineStr"/>
       <c r="R27" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -2582,26 +2777,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K28" t="inlineStr"/>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>2019-2</t>
+        </is>
+      </c>
       <c r="L28" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/jair-hernando-vidal-zuñiga-43a91bb8/</t>
         </is>
       </c>
-      <c r="M28" t="inlineStr">
+      <c r="N28" t="inlineStr">
         <is>
           <t>Analista funcional de aplicacion en Siderurgica de Occidente SA</t>
         </is>
       </c>
-      <c r="N28" t="inlineStr"/>
       <c r="O28" t="inlineStr"/>
       <c r="P28" t="inlineStr"/>
-      <c r="Q28" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q28" t="inlineStr"/>
       <c r="R28" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -2654,18 +2858,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K29" t="inlineStr"/>
-      <c r="L29" t="inlineStr"/>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
       <c r="M29" t="inlineStr"/>
       <c r="N29" t="inlineStr"/>
       <c r="O29" t="inlineStr"/>
       <c r="P29" t="inlineStr"/>
-      <c r="Q29" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q29" t="inlineStr"/>
       <c r="R29" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -2722,26 +2935,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K30" t="inlineStr"/>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>2020-1</t>
+        </is>
+      </c>
       <c r="L30" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/cesar-ceballos-78062337/</t>
         </is>
       </c>
-      <c r="M30" t="inlineStr">
+      <c r="N30" t="inlineStr">
         <is>
           <t>onsultoria y administración en bases de datos ORACLE,PL/SQL. Desarrollador WEB y Móviles.Fundación Centro Colombiano de Estudios Profesionales - FCECEP</t>
         </is>
       </c>
-      <c r="N30" t="inlineStr"/>
       <c r="O30" t="inlineStr"/>
       <c r="P30" t="inlineStr"/>
-      <c r="Q30" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q30" t="inlineStr"/>
       <c r="R30" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -2798,26 +3020,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K31" t="inlineStr"/>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>2020-1</t>
+        </is>
+      </c>
       <c r="L31" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/andres-moreno-collazos-0134081a/</t>
         </is>
       </c>
-      <c r="M31" t="inlineStr">
+      <c r="N31" t="inlineStr">
         <is>
           <t>Ingeniero de Sistemas independiente</t>
         </is>
       </c>
-      <c r="N31" t="inlineStr"/>
       <c r="O31" t="inlineStr"/>
       <c r="P31" t="inlineStr"/>
-      <c r="Q31" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q31" t="inlineStr"/>
       <c r="R31" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -2876,42 +3107,47 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>2020-2</t>
+          <t>2019-1</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/gersonmorera/</t>
         </is>
       </c>
-      <c r="M32" t="inlineStr">
+      <c r="N32" t="inlineStr">
         <is>
           <t>Arquitecto / Lider Tecnico en PRAGMA S.A</t>
         </is>
       </c>
-      <c r="N32" t="inlineStr">
+      <c r="O32" t="inlineStr">
         <is>
           <t xml:space="preserve">“ARQUITECTURA DE REFERENCIA PARA PREVENTA Y POSTVENTA DE
 PROYECTOS DE DESARROLLO DE SOFTWARE”
 </t>
         </is>
       </c>
-      <c r="O32" t="inlineStr">
+      <c r="P32" t="inlineStr">
         <is>
           <t>14 DE ABRIL DE 2020</t>
         </is>
       </c>
-      <c r="P32" t="inlineStr">
+      <c r="Q32" t="inlineStr">
         <is>
           <t>JUAN CARLOS MARTÍNEZ ARIAS</t>
         </is>
       </c>
-      <c r="Q32" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
       <c r="R32" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -2964,18 +3200,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K33" t="inlineStr"/>
-      <c r="L33" t="inlineStr"/>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>2019-2</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
       <c r="M33" t="inlineStr"/>
       <c r="N33" t="inlineStr"/>
       <c r="O33" t="inlineStr"/>
       <c r="P33" t="inlineStr"/>
-      <c r="Q33" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q33" t="inlineStr"/>
       <c r="R33" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3032,26 +3277,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K34" t="inlineStr"/>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
       <c r="L34" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/yiseth-melissa-bedoya-cardona-14194715b/</t>
         </is>
       </c>
-      <c r="M34" t="inlineStr">
+      <c r="N34" t="inlineStr">
         <is>
           <t>Ingeniero de Implementación de Software en Audifarma S.A</t>
         </is>
       </c>
-      <c r="N34" t="inlineStr"/>
       <c r="O34" t="inlineStr"/>
       <c r="P34" t="inlineStr"/>
-      <c r="Q34" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q34" t="inlineStr"/>
       <c r="R34" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3108,26 +3362,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr"/>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
       <c r="L35" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/oscar-fernando-calero-mayor-3a03517b/</t>
         </is>
       </c>
-      <c r="M35" t="inlineStr">
+      <c r="N35" t="inlineStr">
         <is>
           <t>Software Development Engineer en Processoft SAS</t>
         </is>
       </c>
-      <c r="N35" t="inlineStr"/>
       <c r="O35" t="inlineStr"/>
       <c r="P35" t="inlineStr"/>
-      <c r="Q35" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q35" t="inlineStr"/>
       <c r="R35" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3184,26 +3447,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K36" t="inlineStr"/>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
       <c r="L36" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/yuli-sidney-garces-bolañod-1847a3140/</t>
         </is>
       </c>
-      <c r="M36" t="inlineStr">
+      <c r="N36" t="inlineStr">
         <is>
           <t>Desarrollador de software en SENA</t>
         </is>
       </c>
-      <c r="N36" t="inlineStr"/>
       <c r="O36" t="inlineStr"/>
       <c r="P36" t="inlineStr"/>
-      <c r="Q36" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q36" t="inlineStr"/>
       <c r="R36" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3260,26 +3532,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K37" t="inlineStr"/>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>2020-1</t>
+        </is>
+      </c>
       <c r="L37" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/sebastiangilpatino/</t>
         </is>
       </c>
-      <c r="M37" t="inlineStr">
+      <c r="N37" t="inlineStr">
         <is>
           <t>Software engineer</t>
         </is>
       </c>
-      <c r="N37" t="inlineStr"/>
       <c r="O37" t="inlineStr"/>
       <c r="P37" t="inlineStr"/>
-      <c r="Q37" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3332,18 +3613,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M38" t="inlineStr"/>
       <c r="N38" t="inlineStr"/>
       <c r="O38" t="inlineStr"/>
       <c r="P38" t="inlineStr"/>
-      <c r="Q38" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q38" t="inlineStr"/>
       <c r="R38" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3396,18 +3686,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K39" t="inlineStr"/>
-      <c r="L39" t="inlineStr"/>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr"/>
       <c r="P39" t="inlineStr"/>
-      <c r="Q39" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3460,18 +3759,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr"/>
-      <c r="L40" t="inlineStr"/>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr"/>
       <c r="O40" t="inlineStr"/>
       <c r="P40" t="inlineStr"/>
-      <c r="Q40" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q40" t="inlineStr"/>
       <c r="R40" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3524,18 +3832,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K41" t="inlineStr"/>
-      <c r="L41" t="inlineStr"/>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M41" t="inlineStr"/>
       <c r="N41" t="inlineStr"/>
       <c r="O41" t="inlineStr"/>
       <c r="P41" t="inlineStr"/>
-      <c r="Q41" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q41" t="inlineStr"/>
       <c r="R41" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3588,18 +3905,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K42" t="inlineStr"/>
-      <c r="L42" t="inlineStr"/>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr"/>
       <c r="O42" t="inlineStr"/>
       <c r="P42" t="inlineStr"/>
-      <c r="Q42" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q42" t="inlineStr"/>
       <c r="R42" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3652,18 +3978,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K43" t="inlineStr"/>
-      <c r="L43" t="inlineStr"/>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M43" t="inlineStr"/>
       <c r="N43" t="inlineStr"/>
       <c r="O43" t="inlineStr"/>
       <c r="P43" t="inlineStr"/>
-      <c r="Q43" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q43" t="inlineStr"/>
       <c r="R43" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S43" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3716,18 +4051,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M44" t="inlineStr"/>
       <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr"/>
       <c r="P44" t="inlineStr"/>
-      <c r="Q44" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q44" t="inlineStr"/>
       <c r="R44" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S44" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3780,18 +4124,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M45" t="inlineStr"/>
       <c r="N45" t="inlineStr"/>
       <c r="O45" t="inlineStr"/>
       <c r="P45" t="inlineStr"/>
-      <c r="Q45" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q45" t="inlineStr"/>
       <c r="R45" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3844,18 +4197,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M46" t="inlineStr"/>
       <c r="N46" t="inlineStr"/>
       <c r="O46" t="inlineStr"/>
       <c r="P46" t="inlineStr"/>
-      <c r="Q46" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q46" t="inlineStr"/>
       <c r="R46" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3908,18 +4270,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K47" t="inlineStr"/>
-      <c r="L47" t="inlineStr"/>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M47" t="inlineStr"/>
       <c r="N47" t="inlineStr"/>
       <c r="O47" t="inlineStr"/>
       <c r="P47" t="inlineStr"/>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q47" t="inlineStr"/>
       <c r="R47" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -3972,18 +4343,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K48" t="inlineStr"/>
-      <c r="L48" t="inlineStr"/>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M48" t="inlineStr"/>
       <c r="N48" t="inlineStr"/>
       <c r="O48" t="inlineStr"/>
       <c r="P48" t="inlineStr"/>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q48" t="inlineStr"/>
       <c r="R48" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S48" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -4040,26 +4420,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K49" t="inlineStr"/>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
       <c r="L49" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M49" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/breiner-eduardo-hernandez-garcía-780a5563/</t>
         </is>
       </c>
-      <c r="M49" t="inlineStr">
+      <c r="N49" t="inlineStr">
         <is>
           <t>Ingeniero de proyectos</t>
         </is>
       </c>
-      <c r="N49" t="inlineStr"/>
       <c r="O49" t="inlineStr"/>
       <c r="P49" t="inlineStr"/>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q49" t="inlineStr"/>
       <c r="R49" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -4112,18 +4501,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K50" t="inlineStr"/>
-      <c r="L50" t="inlineStr"/>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M50" t="inlineStr"/>
       <c r="N50" t="inlineStr"/>
       <c r="O50" t="inlineStr"/>
       <c r="P50" t="inlineStr"/>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q50" t="inlineStr"/>
       <c r="R50" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S50" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -4176,18 +4574,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K51" t="inlineStr"/>
-      <c r="L51" t="inlineStr"/>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M51" t="inlineStr"/>
       <c r="N51" t="inlineStr"/>
       <c r="O51" t="inlineStr"/>
       <c r="P51" t="inlineStr"/>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q51" t="inlineStr"/>
       <c r="R51" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S51" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -4240,18 +4647,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K52" t="inlineStr"/>
-      <c r="L52" t="inlineStr"/>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M52" t="inlineStr"/>
       <c r="N52" t="inlineStr"/>
       <c r="O52" t="inlineStr"/>
       <c r="P52" t="inlineStr"/>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q52" t="inlineStr"/>
       <c r="R52" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S52" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -4304,18 +4720,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K53" t="inlineStr"/>
-      <c r="L53" t="inlineStr"/>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M53" t="inlineStr"/>
       <c r="N53" t="inlineStr"/>
       <c r="O53" t="inlineStr"/>
       <c r="P53" t="inlineStr"/>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q53" t="inlineStr"/>
       <c r="R53" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -4368,18 +4793,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K54" t="inlineStr"/>
-      <c r="L54" t="inlineStr"/>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="inlineStr"/>
       <c r="O54" t="inlineStr"/>
       <c r="P54" t="inlineStr"/>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q54" t="inlineStr"/>
       <c r="R54" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -4436,26 +4870,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K55" t="inlineStr"/>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
       <c r="L55" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M55" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/dario-leonardo-narvaez-jacome-03984585/</t>
         </is>
       </c>
-      <c r="M55" t="inlineStr">
+      <c r="N55" t="inlineStr">
         <is>
           <t>Validation Engineer</t>
         </is>
       </c>
-      <c r="N55" t="inlineStr"/>
       <c r="O55" t="inlineStr"/>
       <c r="P55" t="inlineStr"/>
-      <c r="Q55" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q55" t="inlineStr"/>
       <c r="R55" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -4508,18 +4951,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K56" t="inlineStr"/>
-      <c r="L56" t="inlineStr"/>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M56" t="inlineStr"/>
       <c r="N56" t="inlineStr"/>
       <c r="O56" t="inlineStr"/>
       <c r="P56" t="inlineStr"/>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q56" t="inlineStr"/>
       <c r="R56" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S56" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -4572,18 +5024,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K57" t="inlineStr"/>
-      <c r="L57" t="inlineStr"/>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M57" t="inlineStr"/>
       <c r="N57" t="inlineStr"/>
       <c r="O57" t="inlineStr"/>
       <c r="P57" t="inlineStr"/>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q57" t="inlineStr"/>
       <c r="R57" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
         <is>
           <t>Si</t>
         </is>
@@ -4636,26 +5097,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K58" t="inlineStr"/>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>2017-1</t>
+        </is>
+      </c>
       <c r="L58" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/mauricio-castrillón-segura-1838695/</t>
         </is>
       </c>
-      <c r="M58" t="inlineStr">
+      <c r="N58" t="inlineStr">
         <is>
           <t>Cafeto software</t>
         </is>
       </c>
-      <c r="N58" t="inlineStr"/>
       <c r="O58" t="inlineStr"/>
       <c r="P58" t="inlineStr"/>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q58" t="inlineStr"/>
       <c r="R58" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S58" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -4710,22 +5180,31 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K59" t="inlineStr"/>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>2017-1</t>
+        </is>
+      </c>
       <c r="L59" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr">
+        <is>
           <t>NO encontada</t>
         </is>
       </c>
-      <c r="M59" t="inlineStr"/>
       <c r="N59" t="inlineStr"/>
       <c r="O59" t="inlineStr"/>
       <c r="P59" t="inlineStr"/>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q59" t="inlineStr"/>
       <c r="R59" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S59" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -4780,26 +5259,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K60" t="inlineStr"/>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>2017-1</t>
+        </is>
+      </c>
       <c r="L60" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/dario-fernando-sussa-carrillo-282bbb9a/</t>
         </is>
       </c>
-      <c r="M60" t="inlineStr">
+      <c r="N60" t="inlineStr">
         <is>
           <t>Jefe de sistemas de normandi</t>
         </is>
       </c>
-      <c r="N60" t="inlineStr"/>
       <c r="O60" t="inlineStr"/>
       <c r="P60" t="inlineStr"/>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q60" t="inlineStr"/>
       <c r="R60" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S60" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -4854,22 +5342,31 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K61" t="inlineStr"/>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>2017-1</t>
+        </is>
+      </c>
       <c r="L61" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M61" t="inlineStr">
+        <is>
           <t>NO encontada</t>
         </is>
       </c>
-      <c r="M61" t="inlineStr"/>
       <c r="N61" t="inlineStr"/>
       <c r="O61" t="inlineStr"/>
       <c r="P61" t="inlineStr"/>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q61" t="inlineStr"/>
       <c r="R61" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S61" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -4926,26 +5423,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K62" t="inlineStr"/>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>2017-2</t>
+        </is>
+      </c>
       <c r="L62" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M62" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/wilmer-bravo-zapata-51357447/</t>
         </is>
       </c>
-      <c r="M62" t="inlineStr">
+      <c r="N62" t="inlineStr">
         <is>
           <t>Senior Software Architect at Modularis</t>
         </is>
       </c>
-      <c r="N62" t="inlineStr"/>
       <c r="O62" t="inlineStr"/>
       <c r="P62" t="inlineStr"/>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q62" t="inlineStr"/>
       <c r="R62" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S62" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5002,22 +5508,31 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K63" t="inlineStr"/>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>2017-2</t>
+        </is>
+      </c>
       <c r="L63" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M63" t="inlineStr">
+        <is>
           <t>NO encontada</t>
         </is>
       </c>
-      <c r="M63" t="inlineStr"/>
       <c r="N63" t="inlineStr"/>
       <c r="O63" t="inlineStr"/>
       <c r="P63" t="inlineStr"/>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q63" t="inlineStr"/>
       <c r="R63" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S63" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5074,22 +5589,31 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K64" t="inlineStr"/>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>2017-2</t>
+        </is>
+      </c>
       <c r="L64" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M64" t="inlineStr">
+        <is>
           <t>NO encontada</t>
         </is>
       </c>
-      <c r="M64" t="inlineStr"/>
       <c r="N64" t="inlineStr"/>
       <c r="O64" t="inlineStr"/>
       <c r="P64" t="inlineStr"/>
-      <c r="Q64" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q64" t="inlineStr"/>
       <c r="R64" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S64" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5146,26 +5670,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K65" t="inlineStr"/>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>2018-1</t>
+        </is>
+      </c>
       <c r="L65" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/maria-alejandra-barbosa-porrras-408ba1180/</t>
         </is>
       </c>
-      <c r="M65" t="inlineStr">
+      <c r="N65" t="inlineStr">
         <is>
           <t>Analista Senior en Banco de Occidente en Banco de Occidente</t>
         </is>
       </c>
-      <c r="N65" t="inlineStr"/>
       <c r="O65" t="inlineStr"/>
       <c r="P65" t="inlineStr"/>
-      <c r="Q65" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q65" t="inlineStr"/>
       <c r="R65" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S65" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5222,26 +5755,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K66" t="inlineStr"/>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>2018-1</t>
+        </is>
+      </c>
       <c r="L66" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M66" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/danielsalasf/</t>
         </is>
       </c>
-      <c r="M66" t="inlineStr">
+      <c r="N66" t="inlineStr">
         <is>
           <t>Software Developer en Mercado Libre</t>
         </is>
       </c>
-      <c r="N66" t="inlineStr"/>
       <c r="O66" t="inlineStr"/>
       <c r="P66" t="inlineStr"/>
-      <c r="Q66" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q66" t="inlineStr"/>
       <c r="R66" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S66" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5298,26 +5840,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K67" t="inlineStr"/>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>2018-1</t>
+        </is>
+      </c>
       <c r="L67" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M67" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/miansamo/</t>
         </is>
       </c>
-      <c r="M67" t="inlineStr">
+      <c r="N67" t="inlineStr">
         <is>
           <t>Senior Software Developer en SproutLoud Media Networks</t>
         </is>
       </c>
-      <c r="N67" t="inlineStr"/>
       <c r="O67" t="inlineStr"/>
       <c r="P67" t="inlineStr"/>
-      <c r="Q67" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q67" t="inlineStr"/>
       <c r="R67" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S67" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5374,26 +5925,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K68" t="inlineStr"/>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>2018-1</t>
+        </is>
+      </c>
       <c r="L68" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/jose-julian-toro-ramirez-099845161/</t>
         </is>
       </c>
-      <c r="M68" t="inlineStr">
+      <c r="N68" t="inlineStr">
         <is>
           <t>Analista sénior en Banco de Occidente</t>
         </is>
       </c>
-      <c r="N68" t="inlineStr"/>
       <c r="O68" t="inlineStr"/>
       <c r="P68" t="inlineStr"/>
-      <c r="Q68" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q68" t="inlineStr"/>
       <c r="R68" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S68" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5450,22 +6010,31 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K69" t="inlineStr"/>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L69" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M69" t="inlineStr">
+        <is>
           <t>No lo encontré</t>
         </is>
       </c>
-      <c r="M69" t="inlineStr"/>
       <c r="N69" t="inlineStr"/>
       <c r="O69" t="inlineStr"/>
       <c r="P69" t="inlineStr"/>
-      <c r="Q69" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q69" t="inlineStr"/>
       <c r="R69" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S69" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5522,26 +6091,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K70" t="inlineStr"/>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L70" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M70" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/juan-carlos-borrero-lópez-14185247/</t>
         </is>
       </c>
-      <c r="M70" t="inlineStr">
+      <c r="N70" t="inlineStr">
         <is>
           <t>Líder de Desarrollo en Universidad del Valle</t>
         </is>
       </c>
-      <c r="N70" t="inlineStr"/>
       <c r="O70" t="inlineStr"/>
       <c r="P70" t="inlineStr"/>
-      <c r="Q70" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q70" t="inlineStr"/>
       <c r="R70" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S70" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5598,26 +6176,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K71" t="inlineStr"/>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L71" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M71" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/ximena-cardenas-rodriguez-148450102/</t>
         </is>
       </c>
-      <c r="M71" t="inlineStr">
+      <c r="N71" t="inlineStr">
         <is>
           <t>Analista de requerimientos y QA en Nuvu</t>
         </is>
       </c>
-      <c r="N71" t="inlineStr"/>
       <c r="O71" t="inlineStr"/>
       <c r="P71" t="inlineStr"/>
-      <c r="Q71" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q71" t="inlineStr"/>
       <c r="R71" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S71" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5674,26 +6261,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K72" t="inlineStr"/>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L72" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M72" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/heidy-lorena-gonzález-b9104271/</t>
         </is>
       </c>
-      <c r="M72" t="inlineStr">
+      <c r="N72" t="inlineStr">
         <is>
           <t>Ingeniera de Requerimientos y SQA</t>
         </is>
       </c>
-      <c r="N72" t="inlineStr"/>
       <c r="O72" t="inlineStr"/>
       <c r="P72" t="inlineStr"/>
-      <c r="Q72" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q72" t="inlineStr"/>
       <c r="R72" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S72" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5750,26 +6346,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K73" t="inlineStr"/>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L73" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/jose-luis-lozano-mosquera/</t>
         </is>
       </c>
-      <c r="M73" t="inlineStr">
+      <c r="N73" t="inlineStr">
         <is>
           <t>Ingeniero de desarrollo de software en TQ Confiable - Tecnoquímicas</t>
         </is>
       </c>
-      <c r="N73" t="inlineStr"/>
       <c r="O73" t="inlineStr"/>
       <c r="P73" t="inlineStr"/>
-      <c r="Q73" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q73" t="inlineStr"/>
       <c r="R73" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S73" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5826,26 +6431,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K74" t="inlineStr"/>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L74" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M74" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/angela-maria-patarroyo-m-771556b4/</t>
         </is>
       </c>
-      <c r="M74" t="inlineStr">
+      <c r="N74" t="inlineStr">
         <is>
           <t>Senior Software Developer at Perficient Latin America</t>
         </is>
       </c>
-      <c r="N74" t="inlineStr"/>
       <c r="O74" t="inlineStr"/>
       <c r="P74" t="inlineStr"/>
-      <c r="Q74" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q74" t="inlineStr"/>
       <c r="R74" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S74" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5902,26 +6516,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K75" t="inlineStr"/>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>2019-1</t>
+        </is>
+      </c>
       <c r="L75" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M75" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/luis-eduardo-aragón-osorio-742727a1/</t>
         </is>
       </c>
-      <c r="M75" t="inlineStr">
+      <c r="N75" t="inlineStr">
         <is>
           <t>Consultor y Arquitecto de software en MVM Ingeniería de software</t>
         </is>
       </c>
-      <c r="N75" t="inlineStr"/>
       <c r="O75" t="inlineStr"/>
       <c r="P75" t="inlineStr"/>
-      <c r="Q75" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q75" t="inlineStr"/>
       <c r="R75" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S75" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -5978,26 +6601,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K76" t="inlineStr"/>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>2019-1</t>
+        </is>
+      </c>
       <c r="L76" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M76" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/jairo-delgado-martinez-337a11106/</t>
         </is>
       </c>
-      <c r="M76" t="inlineStr">
+      <c r="N76" t="inlineStr">
         <is>
           <t>Desarrollador Junior en Xoftix</t>
         </is>
       </c>
-      <c r="N76" t="inlineStr"/>
       <c r="O76" t="inlineStr"/>
       <c r="P76" t="inlineStr"/>
-      <c r="Q76" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q76" t="inlineStr"/>
       <c r="R76" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S76" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6054,26 +6686,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K77" t="inlineStr"/>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>2019-1</t>
+        </is>
+      </c>
       <c r="L77" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M77" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/maria-enith-franco-044ba492/</t>
         </is>
       </c>
-      <c r="M77" t="inlineStr">
+      <c r="N77" t="inlineStr">
         <is>
           <t>Ingeniera de Pruebas GreenSQA</t>
         </is>
       </c>
-      <c r="N77" t="inlineStr"/>
       <c r="O77" t="inlineStr"/>
       <c r="P77" t="inlineStr"/>
-      <c r="Q77" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q77" t="inlineStr"/>
       <c r="R77" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S77" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6130,26 +6771,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K78" t="inlineStr"/>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>2019-1</t>
+        </is>
+      </c>
       <c r="L78" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/andreslrz/</t>
         </is>
       </c>
-      <c r="M78" t="inlineStr">
+      <c r="N78" t="inlineStr">
         <is>
           <t>Analista de ingenieria de software 1 en Personalsoft S.A.S</t>
         </is>
       </c>
-      <c r="N78" t="inlineStr"/>
       <c r="O78" t="inlineStr"/>
       <c r="P78" t="inlineStr"/>
-      <c r="Q78" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q78" t="inlineStr"/>
       <c r="R78" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S78" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6206,26 +6856,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K79" t="inlineStr"/>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>2018-2</t>
+        </is>
+      </c>
       <c r="L79" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/diegohmeneses/</t>
         </is>
       </c>
-      <c r="M79" t="inlineStr">
+      <c r="N79" t="inlineStr">
         <is>
           <t>Director de TIC en Audeed</t>
         </is>
       </c>
-      <c r="N79" t="inlineStr"/>
       <c r="O79" t="inlineStr"/>
       <c r="P79" t="inlineStr"/>
-      <c r="Q79" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q79" t="inlineStr"/>
       <c r="R79" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S79" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6282,22 +6941,31 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K80" t="inlineStr"/>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>2019-2</t>
+        </is>
+      </c>
       <c r="L80" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M80" t="inlineStr">
+        <is>
           <t>NO encontada</t>
         </is>
       </c>
-      <c r="M80" t="inlineStr"/>
       <c r="N80" t="inlineStr"/>
       <c r="O80" t="inlineStr"/>
       <c r="P80" t="inlineStr"/>
-      <c r="Q80" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q80" t="inlineStr"/>
       <c r="R80" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S80" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6354,22 +7022,31 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K81" t="inlineStr"/>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>2019-2</t>
+        </is>
+      </c>
       <c r="L81" t="inlineStr">
         <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="M81" t="inlineStr">
+        <is>
           <t>NO encontada</t>
         </is>
       </c>
-      <c r="M81" t="inlineStr"/>
       <c r="N81" t="inlineStr"/>
       <c r="O81" t="inlineStr"/>
       <c r="P81" t="inlineStr"/>
-      <c r="Q81" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q81" t="inlineStr"/>
       <c r="R81" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S81" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6422,18 +7099,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K82" t="inlineStr"/>
-      <c r="L82" t="inlineStr"/>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>2019-2</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
       <c r="M82" t="inlineStr"/>
       <c r="N82" t="inlineStr"/>
       <c r="O82" t="inlineStr"/>
       <c r="P82" t="inlineStr"/>
-      <c r="Q82" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q82" t="inlineStr"/>
       <c r="R82" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S82" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6490,22 +7176,31 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K83" t="inlineStr"/>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>2020-1</t>
+        </is>
+      </c>
       <c r="L83" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M83" t="inlineStr">
+        <is>
           <t>NO encontada</t>
         </is>
       </c>
-      <c r="M83" t="inlineStr"/>
       <c r="N83" t="inlineStr"/>
       <c r="O83" t="inlineStr"/>
       <c r="P83" t="inlineStr"/>
-      <c r="Q83" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q83" t="inlineStr"/>
       <c r="R83" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S83" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6558,18 +7253,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K84" t="inlineStr"/>
-      <c r="L84" t="inlineStr"/>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M84" t="inlineStr"/>
       <c r="N84" t="inlineStr"/>
       <c r="O84" t="inlineStr"/>
       <c r="P84" t="inlineStr"/>
-      <c r="Q84" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q84" t="inlineStr"/>
       <c r="R84" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S84" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6626,22 +7330,31 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K85" t="inlineStr"/>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>2020-1</t>
+        </is>
+      </c>
       <c r="L85" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M85" t="inlineStr">
+        <is>
           <t>NO encontada</t>
         </is>
       </c>
-      <c r="M85" t="inlineStr"/>
       <c r="N85" t="inlineStr"/>
       <c r="O85" t="inlineStr"/>
       <c r="P85" t="inlineStr"/>
-      <c r="Q85" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q85" t="inlineStr"/>
       <c r="R85" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S85" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6698,26 +7411,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K86" t="inlineStr"/>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>2020-1</t>
+        </is>
+      </c>
       <c r="L86" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M86" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/luis-santiago-osorio-ortiz-02220ab5/</t>
         </is>
       </c>
-      <c r="M86" t="inlineStr">
+      <c r="N86" t="inlineStr">
         <is>
           <t>Ingeniero de desarrollo .Net</t>
         </is>
       </c>
-      <c r="N86" t="inlineStr"/>
       <c r="O86" t="inlineStr"/>
       <c r="P86" t="inlineStr"/>
-      <c r="Q86" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q86" t="inlineStr"/>
       <c r="R86" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S86" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6774,26 +7496,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K87" t="inlineStr"/>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>2020-1</t>
+        </is>
+      </c>
       <c r="L87" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M87" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/jhonatan-vasquez-muñoz-b17886197/</t>
         </is>
       </c>
-      <c r="M87" t="inlineStr">
+      <c r="N87" t="inlineStr">
         <is>
           <t>Quality Assurance Analyst en Yuxi Global</t>
         </is>
       </c>
-      <c r="N87" t="inlineStr"/>
       <c r="O87" t="inlineStr"/>
       <c r="P87" t="inlineStr"/>
-      <c r="Q87" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q87" t="inlineStr"/>
       <c r="R87" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S87" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6850,26 +7581,35 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K88" t="inlineStr"/>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>2020-1</t>
+        </is>
+      </c>
       <c r="L88" t="inlineStr">
         <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="M88" t="inlineStr">
+        <is>
           <t>https://www.linkedin.com/in/harold-william-victoria-sandoval-6b47ba1a6/</t>
         </is>
       </c>
-      <c r="M88" t="inlineStr">
+      <c r="N88" t="inlineStr">
         <is>
           <t>Analista de Desarrollo de Software en Fundación Valle del Lili</t>
         </is>
       </c>
-      <c r="N88" t="inlineStr"/>
       <c r="O88" t="inlineStr"/>
       <c r="P88" t="inlineStr"/>
-      <c r="Q88" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
+      <c r="Q88" t="inlineStr"/>
       <c r="R88" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="S88" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6922,18 +7662,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K89" t="inlineStr"/>
-      <c r="L89" t="inlineStr"/>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M89" t="inlineStr"/>
       <c r="N89" t="inlineStr"/>
       <c r="O89" t="inlineStr"/>
       <c r="P89" t="inlineStr"/>
-      <c r="Q89" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q89" t="inlineStr"/>
       <c r="R89" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S89" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -6986,18 +7735,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K90" t="inlineStr"/>
-      <c r="L90" t="inlineStr"/>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M90" t="inlineStr"/>
       <c r="N90" t="inlineStr"/>
       <c r="O90" t="inlineStr"/>
       <c r="P90" t="inlineStr"/>
-      <c r="Q90" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q90" t="inlineStr"/>
       <c r="R90" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S90" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -7050,18 +7808,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K91" t="inlineStr"/>
-      <c r="L91" t="inlineStr"/>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M91" t="inlineStr"/>
       <c r="N91" t="inlineStr"/>
       <c r="O91" t="inlineStr"/>
       <c r="P91" t="inlineStr"/>
-      <c r="Q91" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q91" t="inlineStr"/>
       <c r="R91" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S91" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -7114,18 +7881,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K92" t="inlineStr"/>
-      <c r="L92" t="inlineStr"/>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M92" t="inlineStr"/>
       <c r="N92" t="inlineStr"/>
       <c r="O92" t="inlineStr"/>
       <c r="P92" t="inlineStr"/>
-      <c r="Q92" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q92" t="inlineStr"/>
       <c r="R92" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S92" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -7178,18 +7954,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K93" t="inlineStr"/>
-      <c r="L93" t="inlineStr"/>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M93" t="inlineStr"/>
       <c r="N93" t="inlineStr"/>
       <c r="O93" t="inlineStr"/>
       <c r="P93" t="inlineStr"/>
-      <c r="Q93" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q93" t="inlineStr"/>
       <c r="R93" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S93" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -7242,18 +8027,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K94" t="inlineStr"/>
-      <c r="L94" t="inlineStr"/>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M94" t="inlineStr"/>
       <c r="N94" t="inlineStr"/>
       <c r="O94" t="inlineStr"/>
       <c r="P94" t="inlineStr"/>
-      <c r="Q94" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q94" t="inlineStr"/>
       <c r="R94" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S94" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -7306,18 +8100,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K95" t="inlineStr"/>
-      <c r="L95" t="inlineStr"/>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M95" t="inlineStr"/>
       <c r="N95" t="inlineStr"/>
       <c r="O95" t="inlineStr"/>
       <c r="P95" t="inlineStr"/>
-      <c r="Q95" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q95" t="inlineStr"/>
       <c r="R95" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S95" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -7370,18 +8173,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K96" t="inlineStr"/>
-      <c r="L96" t="inlineStr"/>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M96" t="inlineStr"/>
       <c r="N96" t="inlineStr"/>
       <c r="O96" t="inlineStr"/>
       <c r="P96" t="inlineStr"/>
-      <c r="Q96" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q96" t="inlineStr"/>
       <c r="R96" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S96" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -7434,18 +8246,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K97" t="inlineStr"/>
-      <c r="L97" t="inlineStr"/>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M97" t="inlineStr"/>
       <c r="N97" t="inlineStr"/>
       <c r="O97" t="inlineStr"/>
       <c r="P97" t="inlineStr"/>
-      <c r="Q97" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q97" t="inlineStr"/>
       <c r="R97" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S97" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -7498,18 +8319,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K98" t="inlineStr"/>
-      <c r="L98" t="inlineStr"/>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M98" t="inlineStr"/>
       <c r="N98" t="inlineStr"/>
       <c r="O98" t="inlineStr"/>
       <c r="P98" t="inlineStr"/>
-      <c r="Q98" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q98" t="inlineStr"/>
       <c r="R98" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S98" t="inlineStr">
         <is>
           <t>No</t>
         </is>
@@ -7562,18 +8392,27 @@
           <t>No</t>
         </is>
       </c>
-      <c r="K99" t="inlineStr"/>
-      <c r="L99" t="inlineStr"/>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>2020-2</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
       <c r="M99" t="inlineStr"/>
       <c r="N99" t="inlineStr"/>
       <c r="O99" t="inlineStr"/>
       <c r="P99" t="inlineStr"/>
-      <c r="Q99" t="inlineStr">
-        <is>
-          <t>Si</t>
-        </is>
-      </c>
+      <c r="Q99" t="inlineStr"/>
       <c r="R99" t="inlineStr">
+        <is>
+          <t>Si</t>
+        </is>
+      </c>
+      <c r="S99" t="inlineStr">
         <is>
           <t>No</t>
         </is>

</xml_diff>